<commit_message>
update new progress for mba dian
</commit_message>
<xml_diff>
--- a/public/templates/uploadprojecttemplate.xlsx
+++ b/public/templates/uploadprojecttemplate.xlsx
@@ -454,7 +454,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -471,7 +471,7 @@
     <col min="10" max="10" width="29.109375" customWidth="1"/>
     <col min="11" max="11" width="27.109375" customWidth="1"/>
     <col min="12" max="12" width="25.109375" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="13" max="13" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">

</xml_diff>